<commit_message>
updated with the lastest version from github
</commit_message>
<xml_diff>
--- a/Assets/images/ImageMap.xlsx
+++ b/Assets/images/ImageMap.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Game Object</t>
   </si>
@@ -53,13 +53,25 @@
     <t>SpinButton</t>
   </si>
   <si>
-    <t>Reel 1</t>
-  </si>
-  <si>
-    <t>Reel 2</t>
-  </si>
-  <si>
-    <t>Reel 3</t>
+    <t>Image 1</t>
+  </si>
+  <si>
+    <t>Image 2</t>
+  </si>
+  <si>
+    <t>Image 3</t>
+  </si>
+  <si>
+    <t>Jackpot Text</t>
+  </si>
+  <si>
+    <t>Credits Text</t>
+  </si>
+  <si>
+    <t>Bet Text</t>
+  </si>
+  <si>
+    <t>Result Text</t>
   </si>
 </sst>
 </file>
@@ -407,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -551,10 +563,78 @@
         <v>44</v>
       </c>
       <c r="D8" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E8" s="2">
         <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
+        <v>65</v>
+      </c>
+      <c r="C9" s="2">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2">
+        <v>293</v>
+      </c>
+      <c r="E9" s="2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2">
+        <v>65</v>
+      </c>
+      <c r="C10" s="2">
+        <v>19</v>
+      </c>
+      <c r="D10" s="2">
+        <v>194</v>
+      </c>
+      <c r="E10" s="2">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2">
+        <v>65</v>
+      </c>
+      <c r="C11" s="2">
+        <v>19</v>
+      </c>
+      <c r="D11" s="2">
+        <v>291</v>
+      </c>
+      <c r="E11" s="2">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2">
+        <v>65</v>
+      </c>
+      <c r="C12" s="2">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2">
+        <v>390</v>
+      </c>
+      <c r="E12" s="2">
+        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>